<commit_message>
Modelagem testes de calculo de dano
</commit_message>
<xml_diff>
--- a/.arquivos/Modelo Mostragem de Dados Warframe.xlsx
+++ b/.arquivos/Modelo Mostragem de Dados Warframe.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9630" windowHeight="7035"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Health</t>
   </si>
@@ -37,13 +36,49 @@
   </si>
   <si>
     <t>ENERGYNG</t>
+  </si>
+  <si>
+    <t>Weapon Calculator</t>
+  </si>
+  <si>
+    <t>Total Damage</t>
+  </si>
+  <si>
+    <t>Puncture</t>
+  </si>
+  <si>
+    <t>Slash</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Void</t>
+  </si>
+  <si>
+    <t>Roar (+50%)</t>
+  </si>
+  <si>
+    <t>Xata Whisper (+17%)</t>
+  </si>
+  <si>
+    <t>Vex Armor (+275%)</t>
+  </si>
+  <si>
+    <t>Lex Prime</t>
+  </si>
+  <si>
+    <t>Heat (Primed HC +165%)</t>
+  </si>
+  <si>
+    <t>Heat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +89,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -87,7 +130,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,22 +489,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:E13"/>
+  <dimension ref="A6:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>100</v>
       </c>
     </row>
@@ -464,7 +513,7 @@
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>50</v>
       </c>
     </row>
@@ -472,7 +521,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>600</v>
       </c>
     </row>
@@ -480,7 +529,7 @@
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>100</v>
       </c>
       <c r="E9" t="s">
@@ -491,7 +540,7 @@
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <f>B6*(B8+300)/300</f>
         <v>300</v>
       </c>
@@ -500,13 +549,214 @@
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3">
+        <f>SUM(B21:B23)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4">
+        <f>B20*2.65</f>
+        <v>397.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3">
+        <f>SUM(B21:B24)</f>
+        <v>547.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="3">
+        <f>B25*1.17</f>
+        <v>640.57499999999993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="4">
+        <f>B24</f>
+        <v>397.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1">
+        <f>B26*0.17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3">
+        <f>SUM(B35:B38)</f>
+        <v>821.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <f>B21*1.5</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" ref="B36:B38" si="0">B22*1.5</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>596.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="3">
+        <f>SUM(B41:B44)</f>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="1">
+        <f>B21*3.75</f>
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1">
+        <f>B22*3.75</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="1">
+        <f>B23*3.75</f>
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1">
+        <f>B24</f>
+        <v>397.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -521,16 +771,4 @@
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>